<commit_message>
Updated tollywood quiz and questions file
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -119,6 +119,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,7 +425,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>